<commit_message>
commitng a christine column chnages in local branch patch 1
</commit_message>
<xml_diff>
--- a/Test Access require.xlsx
+++ b/Test Access require.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\Git\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CF6A14-F122-43EA-942E-DFAE4597E936}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="20736" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Area</t>
   </si>
@@ -317,11 +323,14 @@
 lookersazure\alanleigh</t>
     </r>
   </si>
+  <si>
+    <t>Sexy and amazing woman</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -537,6 +546,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -584,7 +596,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,9 +629,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -652,6 +681,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -827,22 +873,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.44140625" style="24" customWidth="1"/>
     <col min="4" max="4" width="42" style="24" customWidth="1"/>
     <col min="5" max="7" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,7 +908,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="22"/>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -874,7 +920,7 @@
         <v>51</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>50</v>
@@ -883,7 +929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
@@ -903,7 +949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.2" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -917,7 +963,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="42" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
@@ -931,7 +977,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -939,7 +985,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -959,7 +1005,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -979,7 +1025,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -987,7 +1033,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1007,7 +1053,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="223.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="214.8" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
@@ -1027,7 +1073,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="17"/>
       <c r="D12" s="8"/>
@@ -1035,7 +1081,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1049,7 +1095,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>17</v>
       </c>
@@ -1069,7 +1115,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -1077,7 +1123,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>25</v>
       </c>
@@ -1097,7 +1143,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
       <c r="C17" s="4" t="s">
         <v>26</v>
@@ -1109,7 +1155,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
       <c r="C18" s="4" t="s">
         <v>28</v>
@@ -1121,7 +1167,7 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1129,7 +1175,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
         <v>29</v>
       </c>
@@ -1139,7 +1185,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>30</v>
       </c>
@@ -1153,7 +1199,7 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>31</v>
       </c>
@@ -1169,7 +1215,7 @@
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1177,7 +1223,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1185,7 +1231,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
@@ -1197,7 +1243,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>35</v>
       </c>
@@ -1211,7 +1257,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -1219,7 +1265,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>38</v>
       </c>
@@ -1231,7 +1277,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>35</v>
       </c>
@@ -1251,7 +1297,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
@@ -1259,7 +1305,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -1267,7 +1313,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>41</v>
       </c>
@@ -1281,7 +1327,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="6"/>
       <c r="C33" s="23" t="s">
         <v>44</v>
@@ -1293,7 +1339,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="6"/>
       <c r="C34" s="23" t="s">
         <v>46</v>
@@ -1307,31 +1353,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>